<commit_message>
fixes fe and back print dublications on xlxs words loading
</commit_message>
<xml_diff>
--- a/src/state/Domain/verbos.xlsx
+++ b/src/state/Domain/verbos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18040" windowHeight="11960"/>
+    <workbookView windowWidth="25600" windowHeight="12000"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="573">
   <si>
     <t>Infinitvo</t>
   </si>
@@ -809,7 +809,7 @@
 escucharon</t>
   </si>
   <si>
-    <t>Oir</t>
+    <t>Oír</t>
   </si>
   <si>
     <t>Слышать</t>
@@ -1494,10 +1494,48 @@
 volaron</t>
   </si>
   <si>
-    <t>Voler</t>
+    <t>Convertir</t>
   </si>
   <si>
     <t>Становиться</t>
+  </si>
+  <si>
+    <t>convierto,
+conviertes,
+convierte,
+convertimos,
+convertís,
+convierten</t>
+  </si>
+  <si>
+    <t>he convertido,
+has convertido,
+ha convertido,
+hemos convertido,
+habéis convertido,
+han convertido</t>
+  </si>
+  <si>
+    <t>convertiré,
+convertirás,
+convertirá,
+convertiremos,
+convertiréis,
+convertirán</t>
+  </si>
+  <si>
+    <t>convertí,
+convertiste,
+convirtió,
+convertimos,
+convertisteis,
+convirtieron</t>
+  </si>
+  <si>
+    <t>Volver</t>
+  </si>
+  <si>
+    <t>Возвращаться</t>
   </si>
   <si>
     <t>vuelvo,
@@ -1532,12 +1570,6 @@
 volvieron</t>
   </si>
   <si>
-    <t>Volver</t>
-  </si>
-  <si>
-    <t>Возвращаться</t>
-  </si>
-  <si>
     <t>Trasladar</t>
   </si>
   <si>
@@ -1574,6 +1606,2013 @@
 trasladamos,
 trasladasteis,
 trasladaron</t>
+  </si>
+  <si>
+    <t>Buscar</t>
+  </si>
+  <si>
+    <t>Искать</t>
+  </si>
+  <si>
+    <t>busco,
+buscas,
+busca,
+buscamos,
+buscáis,
+buscan</t>
+  </si>
+  <si>
+    <t>he buscado,
+has buscado,
+ha buscado,
+hemos buscado,
+habéis buscado,
+han buscado</t>
+  </si>
+  <si>
+    <t>buscaré,
+buscarás,
+buscará,
+buscaremos,
+buscaréis,
+buscarán</t>
+  </si>
+  <si>
+    <t>busqué,
+buscaste,
+buscó,
+buscamos,
+buscasteis,
+buscaron</t>
+  </si>
+  <si>
+    <t>Nadar</t>
+  </si>
+  <si>
+    <t>Плавать</t>
+  </si>
+  <si>
+    <t>nado,
+nadas,
+nada,
+nadamos,
+nadáis,
+nadan</t>
+  </si>
+  <si>
+    <t>he nadado,
+has nadado,
+ha nadado,
+hemos nadado,
+habéis nadado,
+han nadado</t>
+  </si>
+  <si>
+    <t>nadaré,
+nadarás,
+nadará,
+nadaremos,
+nadaréis,
+nadarán</t>
+  </si>
+  <si>
+    <t>nadé,
+nadaste,
+nadó,
+nadamos,
+nadasteis,
+nadaron</t>
+  </si>
+  <si>
+    <t>Elegir</t>
+  </si>
+  <si>
+    <t>Выбирать</t>
+  </si>
+  <si>
+    <t>elijo,
+eliges,
+elige,
+elegimos,
+elegís,
+eligen</t>
+  </si>
+  <si>
+    <t>he elegido,
+has elegido,
+ha elegido,
+hemos elegido,
+habéis elegido,
+han elegido</t>
+  </si>
+  <si>
+    <t>elegiré,
+elegirás,
+elegirá,
+elegiremos,
+elegiréis,
+elegirán</t>
+  </si>
+  <si>
+    <t>elegí,
+elegiste,
+eligió,
+elegimos,
+elegisteis,
+eligieron</t>
+  </si>
+  <si>
+    <t>Esperar</t>
+  </si>
+  <si>
+    <t>Ждать</t>
+  </si>
+  <si>
+    <t>espero,
+esperas,
+espera,
+esperamos,
+esperáis,
+esperan</t>
+  </si>
+  <si>
+    <t>he esperado,
+has esperado,
+ha esperado,
+hemos esperado,
+habéis esperado,
+han esperado</t>
+  </si>
+  <si>
+    <t>esperaré,
+esperarás,
+esperará,
+esperaremos,
+esperaréis,
+esperarán</t>
+  </si>
+  <si>
+    <t>esperé,
+esperaste,
+esperó,
+esperamos,
+esperasteis,
+esperaron</t>
+  </si>
+  <si>
+    <t>Crear</t>
+  </si>
+  <si>
+    <t>Создавать</t>
+  </si>
+  <si>
+    <t>creo,
+creas,
+crea,
+creamos,
+creáis,
+crean</t>
+  </si>
+  <si>
+    <t>he creado,
+has creado,
+ha creado,
+hemos creado,
+habéis creado,
+han creado</t>
+  </si>
+  <si>
+    <t>crearé,
+crearás,
+creará,
+crearemos,
+crearéis,
+crearán</t>
+  </si>
+  <si>
+    <t>creé,
+creaste,
+creó,
+creamos,
+creasteis,
+crearon</t>
+  </si>
+  <si>
+    <t>Luchar</t>
+  </si>
+  <si>
+    <t>Бороться,драться</t>
+  </si>
+  <si>
+    <t>lucho,
+luchas,
+lucha,
+luchamos,
+lucháis,
+luchan</t>
+  </si>
+  <si>
+    <t>he luchado,
+has luchado,
+ha luchado,
+hemos luchado,
+habéis luchado,
+han luchado</t>
+  </si>
+  <si>
+    <t>lucharé,
+lucharás,
+luchará,
+lucharemos,
+lucharéis,
+lucharán</t>
+  </si>
+  <si>
+    <t>luché,
+luchaste,
+luchó,
+luchamos,
+luchasteis,
+lucharon</t>
+  </si>
+  <si>
+    <t>Tomar</t>
+  </si>
+  <si>
+    <t>Брать</t>
+  </si>
+  <si>
+    <t>tomo,
+tomas,
+toma,
+tomamos,
+tomáis,
+toman</t>
+  </si>
+  <si>
+    <t>he tomado,
+has tomado,
+ha tomado,
+hemos tomado,
+habéis tomado,
+han tomado</t>
+  </si>
+  <si>
+    <t>tomaré,
+tomarás,
+tomará,
+tomaremos,
+tomaréis,
+tomarán</t>
+  </si>
+  <si>
+    <t>tomé,
+tomaste,
+tomó,
+tomamos,
+tomasteis,
+tomaron</t>
+  </si>
+  <si>
+    <t>Enseñar</t>
+  </si>
+  <si>
+    <t>Обучать</t>
+  </si>
+  <si>
+    <t>enseño,
+enseñas,
+enseña,
+enseñamos,
+enseñáis,
+enseñan</t>
+  </si>
+  <si>
+    <t>he enseñado,
+has enseñado,
+ha enseñado,
+hemos enseñado,
+habéis enseñado,
+han enseñado</t>
+  </si>
+  <si>
+    <t>enseñaré,
+enseñarás,
+enseñará,
+enseñaremos,
+enseñaréis,
+enseñarán</t>
+  </si>
+  <si>
+    <t>enseñé,
+enseñaste,
+enseñó,
+enseñamos,
+enseñasteis,
+enseñaron</t>
+  </si>
+  <si>
+    <t>Decir</t>
+  </si>
+  <si>
+    <t>Сказать</t>
+  </si>
+  <si>
+    <t>digo,
+dices,
+dice,
+decimos,
+decís,
+dicen</t>
+  </si>
+  <si>
+    <t>he dicho,
+has dicho,
+ha dicho,
+hemos dicho,
+habéis dicho,
+han dicho</t>
+  </si>
+  <si>
+    <t>diré,
+dirás,
+dirá,
+diremos,
+diréis,
+dirán</t>
+  </si>
+  <si>
+    <t>dije,
+dijiste,
+dijo,
+dijimos,
+dijisteis,
+dijeron</t>
+  </si>
+  <si>
+    <t>Romper</t>
+  </si>
+  <si>
+    <t>Ломать</t>
+  </si>
+  <si>
+    <t>rompo,
+rompes,
+rompe,
+rompemos,
+rompéis,
+rompen</t>
+  </si>
+  <si>
+    <t>he roto,
+has roto,
+ha roto,
+hemos roto,
+habéis roto,
+han roto</t>
+  </si>
+  <si>
+    <t>romperé,
+romperás,
+romperá,
+romperemos,
+romperéis,
+romperán</t>
+  </si>
+  <si>
+    <t>rompí,
+rompiste,
+rompió,
+rompimos,
+rompisteis,
+rompieron</t>
+  </si>
+  <si>
+    <t>Permanecer</t>
+  </si>
+  <si>
+    <t>Останавливать,оставаться</t>
+  </si>
+  <si>
+    <t>permanezco,
+permaneces,
+permanece,
+permanecemos,
+permanecéis,
+permanecen</t>
+  </si>
+  <si>
+    <t>he permanecido,
+has permanecido,
+ha permanecido,
+hemos permanecido,
+habéis permanecido,
+han permanecido</t>
+  </si>
+  <si>
+    <t>permaneceré,
+permanecerás,
+permanecerá,
+permaneceremos,
+permaneceréis,
+permanecerán</t>
+  </si>
+  <si>
+    <t>permanecí,
+permaneciste,
+permaneció,
+permanecimos,
+permanecisteis,
+permanecieron</t>
+  </si>
+  <si>
+    <t>Deber</t>
+  </si>
+  <si>
+    <t>Должен</t>
+  </si>
+  <si>
+    <t>debo,
+debes,
+debe,
+debemos,
+debéis,
+deben</t>
+  </si>
+  <si>
+    <t>he debido,
+has debido,
+ha debido,
+hemos debido,
+habéis debido,
+han debido</t>
+  </si>
+  <si>
+    <t>deberé,
+deberás,
+deberá,
+deberemos,
+deberéis,
+deberán</t>
+  </si>
+  <si>
+    <t>debí,
+debiste,
+debió,
+debimos,
+debisteis,
+debieron</t>
+  </si>
+  <si>
+    <t>Preguntar</t>
+  </si>
+  <si>
+    <t>Спрашивать</t>
+  </si>
+  <si>
+    <t>pregunto,
+preguntas,
+pregunta,
+preguntamos,
+preguntáis,
+preguntan</t>
+  </si>
+  <si>
+    <t>he preguntado,
+has preguntado,
+ha preguntado,
+hemos preguntado,
+habéis preguntado,
+han preguntado</t>
+  </si>
+  <si>
+    <t>preguntaré,
+preguntarás,
+preguntará,
+preguntaremos,
+preguntaréis,
+preguntarán</t>
+  </si>
+  <si>
+    <t>pregunté,
+preguntaste,
+preguntó,
+preguntamos,
+preguntasteis,
+preguntaron</t>
+  </si>
+  <si>
+    <t>Tardar</t>
+  </si>
+  <si>
+    <t>Занимать,ждать</t>
+  </si>
+  <si>
+    <t>tardo,
+tardas,
+tarda,
+tardamos,
+tardáis,
+tardan</t>
+  </si>
+  <si>
+    <t>he tardado,
+has tardado,
+ha tardado,
+hemos tardado,
+habéis tardado,
+han tardado</t>
+  </si>
+  <si>
+    <t>tardaré,
+tardarás,
+tardará,
+tardaremos,
+tardaréis,
+tardarán</t>
+  </si>
+  <si>
+    <t>tardé,
+tardaste,
+tardó,
+tardamos,
+tardasteis,
+tardaron</t>
+  </si>
+  <si>
+    <t>Acabar</t>
+  </si>
+  <si>
+    <t>Заканчивать</t>
+  </si>
+  <si>
+    <t>acabo,
+acabas,
+acaba,
+acabamos,
+acabáis,
+acaban</t>
+  </si>
+  <si>
+    <t>he acabado,
+has acabado,
+ha acabado,
+hemos acabado,
+habéis acabado,
+han acabado</t>
+  </si>
+  <si>
+    <t>acabaré,
+acabarás,
+acabará,
+acabaremos,
+acabaréis,
+acabarán</t>
+  </si>
+  <si>
+    <t>acabé,
+acabaste,
+acabó,
+acabamos,
+acabasteis,
+acabaron</t>
+  </si>
+  <si>
+    <t>Traer</t>
+  </si>
+  <si>
+    <t>Приносить,привезти,вернуть</t>
+  </si>
+  <si>
+    <t>traigo,
+traes,
+trae,
+traemos,
+traéis,
+traen</t>
+  </si>
+  <si>
+    <t>he traído,
+has traído,
+ha traído,
+hemos traído,
+habéis traído,
+han traído</t>
+  </si>
+  <si>
+    <t>traeré,
+traerás,
+traerá,
+traeremos,
+traeréis,
+traerán</t>
+  </si>
+  <si>
+    <t>traje,
+trajiste,
+trajo,
+trajimos,
+trajisteis,
+trajeron</t>
+  </si>
+  <si>
+    <t>Dirigir</t>
+  </si>
+  <si>
+    <t>Управлять,руководить</t>
+  </si>
+  <si>
+    <t>dirijo,
+diriges,
+dirige,
+dirigimos,
+dirigís,
+dirigen</t>
+  </si>
+  <si>
+    <t>he dirigido,
+has dirigido,
+ha dirigido,
+hemos dirigido,
+habéis dirigido,
+han dirigido</t>
+  </si>
+  <si>
+    <t>dirigiré,
+dirigirás,
+dirigirá,
+dirigiremos,
+dirigiréis,
+dirigirán</t>
+  </si>
+  <si>
+    <t>dirigí,
+dirigiste,
+dirigió,
+dirigimos,
+dirigisteis,
+dirigieron</t>
+  </si>
+  <si>
+    <t>Gustar</t>
+  </si>
+  <si>
+    <t>Нравиться,любить</t>
+  </si>
+  <si>
+    <t>gusto,
+gustas,
+gusta,
+gustamos,
+gustáis,
+gustan</t>
+  </si>
+  <si>
+    <t>he gustado,
+has gustado,
+ha gustado,
+hemos gustado,
+habéis gustado,
+han gustado</t>
+  </si>
+  <si>
+    <t>gustaré,
+gustarás,
+gustará,
+gustaremos,
+gustaréis,
+gustarán</t>
+  </si>
+  <si>
+    <t>gusté,
+gustaste,
+gustó,
+gustamos,
+gustasteis,
+gustaron</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cumplir </t>
+  </si>
+  <si>
+    <t>Соблюдать,выполнять,исполнить</t>
+  </si>
+  <si>
+    <t>cumplo,
+cumples,
+cumple,
+cumplimos,
+cumplís,
+cumplen</t>
+  </si>
+  <si>
+    <t>he cumplido,
+has cumplido,
+ha cumplido,
+hemos cumplido,
+habéis cumplido,
+han cumplido</t>
+  </si>
+  <si>
+    <t>cumpliré,
+cumplirás,
+cumplirá,
+cumpliremos,
+cumpliréis,
+cumplirán</t>
+  </si>
+  <si>
+    <t>cumplí,
+cumpliste,
+cumplió,
+cumplimos,
+cumplisteis,
+cumplieron</t>
+  </si>
+  <si>
+    <t>Intentar</t>
+  </si>
+  <si>
+    <t>Попробовать,попытаться</t>
+  </si>
+  <si>
+    <t>intento,
+intentas,
+intenta,
+intentamos,
+intentáis,
+intentan</t>
+  </si>
+  <si>
+    <t>he intentado,
+has intentado,
+ha intentado,
+hemos intentado,
+habéis intentado,
+han intentado</t>
+  </si>
+  <si>
+    <t>intentaré,
+intentarás,
+intentará,
+intentaremos,
+intentaréis,
+intentarán</t>
+  </si>
+  <si>
+    <t>intenté,
+intentaste,
+intentó,
+intentamos,
+intentasteis,
+intentaron</t>
+  </si>
+  <si>
+    <t>Usar</t>
+  </si>
+  <si>
+    <t>Использовать</t>
+  </si>
+  <si>
+    <t>uso,
+usas,
+usa,
+usamos,
+usáis,
+usan</t>
+  </si>
+  <si>
+    <t>he usado,
+has usado,
+ha usado,
+hemos usado,
+habéis usado,
+han usado</t>
+  </si>
+  <si>
+    <t>usaré,
+usarás,
+usará,
+usaremos,
+usaréis,
+usarán</t>
+  </si>
+  <si>
+    <t>usé,
+usaste,
+usó,
+usamos,
+usasteis,
+usaron</t>
+  </si>
+  <si>
+    <t>Llegar</t>
+  </si>
+  <si>
+    <t>Прибывать,приехать,добраться</t>
+  </si>
+  <si>
+    <t>llego,
+llegas,
+llega,
+llegamos,
+llegáis,
+llegan</t>
+  </si>
+  <si>
+    <t>he llegado,
+has llegado,
+ha llegado,
+hemos llegado,
+habéis llegado,
+han llegado</t>
+  </si>
+  <si>
+    <t>llegaré,
+llegarás,
+llegará,
+llegaremos,
+llegaréis,
+llegarán</t>
+  </si>
+  <si>
+    <t>llegué,
+llegaste,
+llegó,
+llegamos,
+llegasteis,
+llegaron</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creer </t>
+  </si>
+  <si>
+    <t>Верить,поверить</t>
+  </si>
+  <si>
+    <t>creo,
+crees,
+cree,
+creemos,
+creéis,
+creen</t>
+  </si>
+  <si>
+    <t>he creído,
+has creído,
+ha creído,
+hemos creído,
+habéis creído,
+han creído</t>
+  </si>
+  <si>
+    <t>creeré,
+creerás,
+creerá,
+creeremos,
+creeréis,
+creerán</t>
+  </si>
+  <si>
+    <t xml:space="preserve">creí,
+creíste,
+creyó,
+creímos,
+creísteis,
+creyeron
+</t>
+  </si>
+  <si>
+    <t>Ocurrir</t>
+  </si>
+  <si>
+    <t>Происходить</t>
+  </si>
+  <si>
+    <t>ocurro,
+ocurres,
+ocurre,
+ocurrimos,
+ocurrís,
+ocurren</t>
+  </si>
+  <si>
+    <t>he ocurrido,
+has ocurrido,
+ha ocurrido,
+hemos ocurrido,
+habéis ocurrido,
+han ocurrido</t>
+  </si>
+  <si>
+    <t>ocurriré,
+ocurrirás,
+ocurrirá,
+ocurriremos,
+ocurriréis,
+ocurrirán</t>
+  </si>
+  <si>
+    <t>ocurrí,
+ocurriste,
+ocurrió,
+ocurrimos,
+ocurristeis,
+ocurrieron</t>
+  </si>
+  <si>
+    <t>Entender</t>
+  </si>
+  <si>
+    <t>Понимать</t>
+  </si>
+  <si>
+    <t>entiendo,
+entiendes,
+entiende,
+entendemos,
+entendéis,
+entienden</t>
+  </si>
+  <si>
+    <t>he entendido,
+has entendido,
+ha entendido,
+hemos entendido,
+habéis entendido,
+han entendido</t>
+  </si>
+  <si>
+    <t>entenderé,
+entenderás,
+entenderá,
+entenderemos,
+entenderéis,
+entenderán</t>
+  </si>
+  <si>
+    <t>entendí,
+entendiste,
+entendió,
+entendimos,
+entendisteis,
+entendieron</t>
+  </si>
+  <si>
+    <t>Permitir</t>
+  </si>
+  <si>
+    <t>Позволять</t>
+  </si>
+  <si>
+    <t>permito,
+permites,
+permite,
+permitimos,
+permitís,
+permiten</t>
+  </si>
+  <si>
+    <t>he permitido,
+has permitido,
+ha permitido,
+hemos permitido,
+habéis permitido,
+han permitido</t>
+  </si>
+  <si>
+    <t>permitiré,
+permitirás,
+permitirá,
+permitiremos,
+permitiréis,
+permitirán</t>
+  </si>
+  <si>
+    <t>permití,
+permitiste,
+permitió,
+permitimos,
+permitisteis,
+permitieron</t>
+  </si>
+  <si>
+    <t>Sacar</t>
+  </si>
+  <si>
+    <t>Вынимать</t>
+  </si>
+  <si>
+    <t>saco,
+sacas,
+saca,
+sacamos,
+sacáis,
+sacan</t>
+  </si>
+  <si>
+    <t>he sacado,
+has sacado,
+ha sacado,
+hemos sacado,
+habéis sacado,
+han sacado</t>
+  </si>
+  <si>
+    <t>sacaré,
+sacarás,
+sacará,
+sacaremos,
+sacaréis,
+sacarán</t>
+  </si>
+  <si>
+    <t>saqué,
+sacaste,
+sacó,
+sacamos,
+sacasteis,
+sacaron</t>
+  </si>
+  <si>
+    <t>Suponer</t>
+  </si>
+  <si>
+    <t>Предполагать</t>
+  </si>
+  <si>
+    <t>supongo,
+supones,
+supone,
+suponemos,
+suponéis,
+suponen</t>
+  </si>
+  <si>
+    <t>he supuesto,
+has supuesto,
+ha supuesto,
+hemos supuesto,
+habéis supuesto,
+han supuesto</t>
+  </si>
+  <si>
+    <t>supondré,
+supondrás,
+supondrá,
+supondremos,
+supondréis,
+supondrán</t>
+  </si>
+  <si>
+    <t>supuse,
+supusiste,
+supuso,
+supusimos,
+supusisteis,
+supusieron</t>
+  </si>
+  <si>
+    <t>Explicar</t>
+  </si>
+  <si>
+    <t>Объяснять</t>
+  </si>
+  <si>
+    <t>explico,
+explicas,
+explica,
+explicamos,
+explicáis,
+explican</t>
+  </si>
+  <si>
+    <t>he explicado,
+has explicado,
+ha explicado,
+hemos explicado,
+habéis explicado,
+han explicado</t>
+  </si>
+  <si>
+    <t>explicaré,
+explicarás,
+explicará,
+explicaremos,
+explicaréis,
+explicarán</t>
+  </si>
+  <si>
+    <t>expliqué,
+explicaste,
+explicó,
+explicamos,
+explicasteis,
+explicaron</t>
+  </si>
+  <si>
+    <t>Tocar</t>
+  </si>
+  <si>
+    <t>трогать,играть на инструменте</t>
+  </si>
+  <si>
+    <t>toco,
+tocas,
+toca,
+tocamos,
+tocáis,
+tocan</t>
+  </si>
+  <si>
+    <t>he tocado,
+has tocado,
+ha tocado,
+hemos tocado,
+habéis tocado,
+han tocado</t>
+  </si>
+  <si>
+    <t>tocaré,
+tocarás,
+tocará,
+tocaremos,
+tocaréis,
+tocarán</t>
+  </si>
+  <si>
+    <t>toqué,
+tocaste,
+tocó,
+tocamos,
+tocasteis,
+tocaron</t>
+  </si>
+  <si>
+    <t>Ayudar</t>
+  </si>
+  <si>
+    <t>помогать</t>
+  </si>
+  <si>
+    <t>ayudo,
+ayudas,
+ayuda,
+ayudamos,
+ayudáis,
+ayudan</t>
+  </si>
+  <si>
+    <t>he ayudado,
+has ayudado,
+ha ayudado,
+hemos ayudado,
+habéis ayudado,
+han ayudado</t>
+  </si>
+  <si>
+    <t>ayudaré,
+ayudarás,
+ayudará,
+ayudaremos,
+ayudaréis,
+ayudarán</t>
+  </si>
+  <si>
+    <t>ayudé,
+ayudaste,
+ayudó,
+ayudamos,
+ayudasteis,
+ayudaron</t>
+  </si>
+  <si>
+    <t>Pedir</t>
+  </si>
+  <si>
+    <t>Просить</t>
+  </si>
+  <si>
+    <t>pido,
+pides,
+pide,
+pedimos,
+pedís,
+piden</t>
+  </si>
+  <si>
+    <t>he pedido,
+has pedido,
+ha pedido,
+hemos pedido,
+habéis pedido,
+han pedido</t>
+  </si>
+  <si>
+    <t>pediré,
+pedirás,
+pedirá,
+pediremos,
+pediréis,
+pedirán</t>
+  </si>
+  <si>
+    <t>pedí,
+pediste,
+pidió,
+pedimos,
+pedisteis,
+pidieron</t>
+  </si>
+  <si>
+    <t>Conducir</t>
+  </si>
+  <si>
+    <t>водить,водить машину</t>
+  </si>
+  <si>
+    <t>conduzco,
+conduces,
+conduce,
+conducimos,
+conducís,
+conducen</t>
+  </si>
+  <si>
+    <t>he conducido,
+has conducido,
+ha conducido,
+hemos conducido,
+habéis conducido,
+han conducido</t>
+  </si>
+  <si>
+    <t>conduciré,
+conducirás,
+conducirá,
+conduciremos,
+conduciréis,
+conducirán</t>
+  </si>
+  <si>
+    <t>conduje,
+condujiste,
+condujo,
+condujimos,
+condujisteis,
+condujeron</t>
+  </si>
+  <si>
+    <t>Incluir</t>
+  </si>
+  <si>
+    <t>Включать</t>
+  </si>
+  <si>
+    <t>incluyo,
+incluyes,
+incluye,
+incluimos,
+incluís,
+incluyen</t>
+  </si>
+  <si>
+    <t>he incluido,
+has incluido,
+ha incluido,
+hemos incluido,
+habéis incluido,
+han incluido</t>
+  </si>
+  <si>
+    <t>incluiré,
+incluirás,
+incluirá,
+incluiremos,
+incluiréis,
+incluirán</t>
+  </si>
+  <si>
+    <t>incluí,
+incluiste,
+incluyó,
+incluimos,
+incluisteis,
+incluyeron</t>
+  </si>
+  <si>
+    <t>Atraversar</t>
+  </si>
+  <si>
+    <t>Переходить</t>
+  </si>
+  <si>
+    <t>atravieso,
+atraviesas,
+atraviesa,
+atravesamos,
+atravesáis,
+atraviesan</t>
+  </si>
+  <si>
+    <t>he atravesado,
+has atravesado,
+ha atravesado,
+hemos atravesado,
+habéis atravesado,
+han atravesado</t>
+  </si>
+  <si>
+    <t>atravesaré,
+atravesarás,
+atravesará,
+atravesaremos,
+atravesaréis,
+atravesarán</t>
+  </si>
+  <si>
+    <t>atravesé,
+atravesaste,
+atravesó,
+atravesamos,
+atravesasteis,
+atravesaron</t>
+  </si>
+  <si>
+    <t>Tener</t>
+  </si>
+  <si>
+    <t>Иметь</t>
+  </si>
+  <si>
+    <t>tengo,
+tienes,
+tiene,
+tenemos,
+tenéis,
+tienen</t>
+  </si>
+  <si>
+    <t>he tenido,
+has tenido,
+ha tenido,
+hemos tenido,
+habéis tenido,
+han tenido</t>
+  </si>
+  <si>
+    <t>tendré,
+tendrás,
+tendrá,
+tendremos,
+tendréis,
+tendrán</t>
+  </si>
+  <si>
+    <t>tuve,
+tuviste,
+tuvo,
+tuvimos,
+tuvisteis,
+tuvieron</t>
+  </si>
+  <si>
+    <t>Ir</t>
+  </si>
+  <si>
+    <t>Идти</t>
+  </si>
+  <si>
+    <t>voy,
+vas,
+va,
+vamos,
+vais,
+van</t>
+  </si>
+  <si>
+    <t>he ido,
+has ido,
+ha ido,
+hemos ido,
+habéis ido,
+han ido</t>
+  </si>
+  <si>
+    <t>iré,
+irás,
+irá,
+iremos,
+iréis,
+irán</t>
+  </si>
+  <si>
+    <t>fui,
+fuiste,
+fue,
+fuimos,
+fuisteis,
+fueron</t>
+  </si>
+  <si>
+    <t>Caer</t>
+  </si>
+  <si>
+    <t>Падать</t>
+  </si>
+  <si>
+    <t>caigo,
+caes,
+cae,
+caemos,
+caéis,
+caen</t>
+  </si>
+  <si>
+    <t>he caído,
+has caído,
+ha caído,
+hemos caído,
+habéis caído,
+han caído</t>
+  </si>
+  <si>
+    <t>caeré,
+caerás,
+caerá,
+caeremos,
+caeréis,
+caerán</t>
+  </si>
+  <si>
+    <t>caí,
+caíste,
+cayó,
+caímos,
+caísteis,
+cayeron</t>
+  </si>
+  <si>
+    <t>Correr</t>
+  </si>
+  <si>
+    <t>Бежать</t>
+  </si>
+  <si>
+    <t>corro,
+corres,
+corre,
+corremos,
+corréis,
+corren</t>
+  </si>
+  <si>
+    <t>he corrido,
+has corrido,
+ha corrido,
+hemos corrido,
+habéis corrido,
+han corrido</t>
+  </si>
+  <si>
+    <t>correré,
+correrás,
+correrá,
+correremos,
+correréis,
+correrán</t>
+  </si>
+  <si>
+    <t>corrí,
+corriste,
+corrió,
+corrimos,
+corristeis,
+corrieron</t>
+  </si>
+  <si>
+    <t>Dejar</t>
+  </si>
+  <si>
+    <t>Оставлять</t>
+  </si>
+  <si>
+    <t>dejo,
+dejas,
+deja,
+dejamos,
+dejáis,
+dejan</t>
+  </si>
+  <si>
+    <t>he dejado,
+has dejado,
+ha dejado,
+hemos dejado,
+habéis dejado,
+han dejado</t>
+  </si>
+  <si>
+    <t>dejaré,
+dejarás,
+dejará,
+dejaremos,
+dejaréis,
+dejarán</t>
+  </si>
+  <si>
+    <t>dejé,
+dejaste,
+dejó,
+dejamos,
+dejasteis,
+dejaron</t>
+  </si>
+  <si>
+    <t>Estudiar</t>
+  </si>
+  <si>
+    <t>Изучать</t>
+  </si>
+  <si>
+    <t>estudio,
+estudias,
+estudia,
+estudiamos,
+estudiáis,
+estudian</t>
+  </si>
+  <si>
+    <t>he estudiado,
+has estudiado,
+ha estudiado,
+hemos estudiado,
+habéis estudiado,
+han estudiado</t>
+  </si>
+  <si>
+    <t>estudiaré,
+estudiarás,
+estudiará,
+estudiaremos,
+estudiaréis,
+estudiarán</t>
+  </si>
+  <si>
+    <t>estudié,
+estudiaste,
+estudió,
+estudiamos,
+estudiasteis,
+estudiaron</t>
+  </si>
+  <si>
+    <t>Formar</t>
+  </si>
+  <si>
+    <t>Форматировать,зарабатывать</t>
+  </si>
+  <si>
+    <t>formo,
+formas,
+forma,
+formamos,
+formáis,
+forman</t>
+  </si>
+  <si>
+    <t>he formado,
+has formado,
+ha formado,
+hemos formado,
+habéis formado,
+han formado</t>
+  </si>
+  <si>
+    <t>formaré,
+formarás,
+formará,
+formaremos,
+formaréis,
+formarán</t>
+  </si>
+  <si>
+    <t>formé,
+formaste,
+formó,
+formamos,
+formasteis,
+formaron</t>
+  </si>
+  <si>
+    <t>Lograr</t>
+  </si>
+  <si>
+    <t>Добиваться</t>
+  </si>
+  <si>
+    <t>logro,
+logras,
+logra,
+logramos,
+lográis,
+logran</t>
+  </si>
+  <si>
+    <t>he logrado,
+has logrado,
+ha logrado,
+hemos logrado,
+habéis logrado,
+han logrado</t>
+  </si>
+  <si>
+    <t>lograré,
+lograrás,
+logrará,
+lograremos,
+lograréis,
+lograrán</t>
+  </si>
+  <si>
+    <t>logré,
+lograste,
+logró,
+logramos,
+lograsteis,
+lograron</t>
+  </si>
+  <si>
+    <t>Necesitar</t>
+  </si>
+  <si>
+    <t>Нуждаться</t>
+  </si>
+  <si>
+    <t>necesito,
+necesitas,
+necesita,
+necesitamos,
+necesitáis,
+necesitan</t>
+  </si>
+  <si>
+    <t>he necesitado,
+has necesitado,
+ha necesitado,
+hemos necesitado,
+habéis necesitado,
+han necesitado</t>
+  </si>
+  <si>
+    <t>necesitaré,
+necesitarás,
+necesitará,
+necesitaremos,
+necesitaréis,
+necesitarán</t>
+  </si>
+  <si>
+    <t>necesité,
+necesitaste,
+necesitó,
+necesitamos,
+necesitasteis,
+necesitaron</t>
+  </si>
+  <si>
+    <t>Perder</t>
+  </si>
+  <si>
+    <t>Терять</t>
+  </si>
+  <si>
+    <t>pierdo,
+pierdes,
+pierde,
+perdemos,
+perdéis,
+pierden</t>
+  </si>
+  <si>
+    <t>he perdido,
+has perdido,
+ha perdido,
+hemos perdido,
+habéis perdido,
+han perdido</t>
+  </si>
+  <si>
+    <t>perderé,
+perderás,
+perderá,
+perderemos,
+perderéis,
+perderán</t>
+  </si>
+  <si>
+    <t>perdí,
+perdiste,
+perdió,
+perdimos,
+perdisteis,
+perdieron</t>
+  </si>
+  <si>
+    <t>Poner</t>
+  </si>
+  <si>
+    <t>Поместить,положить</t>
+  </si>
+  <si>
+    <t>pongo,
+pones,
+pone,
+ponemos,
+ponéis,
+ponen</t>
+  </si>
+  <si>
+    <t>he puesto,
+has puesto,
+ha puesto,
+hemos puesto,
+habéis puesto,
+han puesto</t>
+  </si>
+  <si>
+    <t>pondré,
+pondrás,
+pondrá,
+pondremos,
+pondréis,
+pondrán</t>
+  </si>
+  <si>
+    <t>puse,
+pusiste,
+puso,
+pusimos,
+pusisteis,
+pusieron</t>
+  </si>
+  <si>
+    <t>Reconocer</t>
+  </si>
+  <si>
+    <t>Признавать</t>
+  </si>
+  <si>
+    <t>reconozco,
+reconoces,
+reconoce,
+reconocemos,
+reconocéis,
+reconocen</t>
+  </si>
+  <si>
+    <t>he reconocido,
+has reconocido,
+ha reconocido,
+hemos reconocido,
+habéis reconocido,
+han reconocido</t>
+  </si>
+  <si>
+    <t>reconoceré,
+reconocerás,
+reconocerá,
+reconoceremos,
+reconoceréis,
+reconocerán</t>
+  </si>
+  <si>
+    <t>reconocí,
+reconociste,
+reconoció,
+reconocimos,
+reconocisteis,
+reconocieron</t>
+  </si>
+  <si>
+    <t>Partir</t>
+  </si>
+  <si>
+    <t>делить,разделять</t>
+  </si>
+  <si>
+    <t>parto,
+partes,
+parte,
+partimos,
+partís,
+parten</t>
+  </si>
+  <si>
+    <t>he partido,
+has partido,
+ha partido,
+hemos partido,
+habéis partido,
+han partido</t>
+  </si>
+  <si>
+    <t>partiré,
+partirás,
+partirá,
+partiremos,
+partiréis,
+partirán</t>
+  </si>
+  <si>
+    <t>partí,
+partiste,
+partió,
+partimos,
+partisteis,
+partieron</t>
+  </si>
+  <si>
+    <t>Pasar</t>
+  </si>
+  <si>
+    <t>Проходить,перемещать</t>
+  </si>
+  <si>
+    <t>paso,
+pasas,
+pasa,
+pasamos,
+pasáis,
+pasan</t>
+  </si>
+  <si>
+    <t>he pasado,
+has pasado,
+ha pasado,
+hemos pasado,
+habéis pasado,
+han pasado</t>
+  </si>
+  <si>
+    <t>pasaré,
+pasarás,
+pasará,
+pasaremos,
+pasaréis,
+pasarán</t>
+  </si>
+  <si>
+    <t>pasé,
+pasaste,
+pasó,
+pasamos,
+pasasteis,
+pasaron</t>
+  </si>
+  <si>
+    <t>Mantener</t>
+  </si>
+  <si>
+    <t>Поддерживать</t>
+  </si>
+  <si>
+    <t>mantengo,
+mantienes,
+mantiene,
+mantenemos,
+mantenéis,
+mantienen</t>
+  </si>
+  <si>
+    <t>he mantenido,
+has mantenido,
+ha mantenido,
+hemos mantenido,
+habéis mantenido,
+han mantenido</t>
+  </si>
+  <si>
+    <t>mantendré,
+mantendrás,
+mantendrá,
+mantendremos,
+mantendréis,
+mantendrán</t>
+  </si>
+  <si>
+    <t>mantuve,
+mantuviste,
+mantuvo,
+mantuvimos,
+mantuvisteis,
+mantuvieron</t>
+  </si>
+  <si>
+    <t>Ser</t>
+  </si>
+  <si>
+    <t>Быть</t>
+  </si>
+  <si>
+    <t>soy,
+eres,
+es,
+somos,
+sois,
+son</t>
+  </si>
+  <si>
+    <t>he sido,
+has sido,
+ha sido,
+hemos sido,
+habéis sido,
+han sido</t>
+  </si>
+  <si>
+    <t>seré,
+serás,
+será,
+seremos,
+seréis,
+serán</t>
+  </si>
+  <si>
+    <t>Comparar</t>
+  </si>
+  <si>
+    <t>Сравнивать</t>
+  </si>
+  <si>
+    <t>comparo,
+comparas,
+compara,
+comparamos,
+comparáis,
+comparan</t>
+  </si>
+  <si>
+    <t>he comparado,
+has comparado,
+ha comparado,
+hemos comparado,
+habéis comparado,
+han comparado</t>
+  </si>
+  <si>
+    <t>compararé,
+compararás,
+comparará,
+compararemos,
+compararéis,
+compararán</t>
+  </si>
+  <si>
+    <t>comparé,
+comparaste,
+comparó,
+comparamos,
+comparasteis,
+compararon</t>
+  </si>
+  <si>
+    <t>Oler</t>
+  </si>
+  <si>
+    <t>Пахнуть</t>
+  </si>
+  <si>
+    <t>huelo,
+hueles,
+huele,
+olemos,
+oléis,
+huelen</t>
+  </si>
+  <si>
+    <t>he olido,
+has olido,
+ha olido,
+hemos olido,
+habéis olido,
+han olido</t>
+  </si>
+  <si>
+    <t>oleré,
+olerás,
+olerá,
+oleremos,
+oleréis,
+olerán</t>
+  </si>
+  <si>
+    <t>olí,
+oliste,
+olió,
+olimos,
+olisteis,
+olieron</t>
   </si>
   <si>
     <t>familia,nouns</t>
@@ -2213,7 +4252,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2225,7 +4264,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2701,15 +4739,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="F101" sqref="F101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6272727272727" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="5"/>
   <cols>
-    <col min="2" max="2" width="29.6363636363636" customWidth="1"/>
+    <col min="2" max="2" width="31.0909090909091" customWidth="1"/>
     <col min="3" max="3" width="32.7272727272727" customWidth="1"/>
     <col min="4" max="4" width="21.9090909090909" customWidth="1"/>
     <col min="5" max="5" width="16.9090909090909" customWidth="1"/>
@@ -3524,43 +5562,1097 @@
         <v>241</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="42" ht="93" customHeight="1" spans="1:6">
       <c r="A42" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="B42" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="43" customHeight="1" spans="6:6">
-      <c r="F43" s="5"/>
-    </row>
-    <row r="44" customHeight="1" spans="6:6">
-      <c r="F44" s="5"/>
+        <v>251</v>
+      </c>
+    </row>
+    <row r="43" ht="81" customHeight="1" spans="1:6">
+      <c r="A43" t="s">
+        <v>252</v>
+      </c>
+      <c r="B43" t="s">
+        <v>253</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="44" ht="84" customHeight="1" spans="1:6">
+      <c r="A44" t="s">
+        <v>258</v>
+      </c>
+      <c r="B44" t="s">
+        <v>259</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="45" ht="81" customHeight="1" spans="1:6">
+      <c r="A45" t="s">
+        <v>264</v>
+      </c>
+      <c r="B45" t="s">
+        <v>265</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="46" ht="88" customHeight="1" spans="1:6">
+      <c r="A46" t="s">
+        <v>270</v>
+      </c>
+      <c r="B46" t="s">
+        <v>271</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="47" ht="78" customHeight="1" spans="1:6">
+      <c r="A47" t="s">
+        <v>276</v>
+      </c>
+      <c r="B47" t="s">
+        <v>277</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="48" ht="81" customHeight="1" spans="1:6">
+      <c r="A48" t="s">
+        <v>282</v>
+      </c>
+      <c r="B48" t="s">
+        <v>283</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="49" ht="76" customHeight="1" spans="1:6">
+      <c r="A49" t="s">
+        <v>288</v>
+      </c>
+      <c r="B49" t="s">
+        <v>289</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="50" ht="80" customHeight="1" spans="1:6">
+      <c r="A50" t="s">
+        <v>294</v>
+      </c>
+      <c r="B50" t="s">
+        <v>295</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="51" ht="83" customHeight="1" spans="1:6">
+      <c r="A51" t="s">
+        <v>300</v>
+      </c>
+      <c r="B51" t="s">
+        <v>301</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="52" ht="76" customHeight="1" spans="1:6">
+      <c r="A52" t="s">
+        <v>306</v>
+      </c>
+      <c r="B52" t="s">
+        <v>307</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="53" ht="83" customHeight="1" spans="1:6">
+      <c r="A53" t="s">
+        <v>312</v>
+      </c>
+      <c r="B53" t="s">
+        <v>313</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="54" ht="79" customHeight="1" spans="1:6">
+      <c r="A54" t="s">
+        <v>318</v>
+      </c>
+      <c r="B54" t="s">
+        <v>319</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="55" ht="83" customHeight="1" spans="1:6">
+      <c r="A55" t="s">
+        <v>324</v>
+      </c>
+      <c r="B55" t="s">
+        <v>325</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="56" ht="80" customHeight="1" spans="1:6">
+      <c r="A56" t="s">
+        <v>330</v>
+      </c>
+      <c r="B56" t="s">
+        <v>331</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="57" ht="80" customHeight="1" spans="1:6">
+      <c r="A57" t="s">
+        <v>336</v>
+      </c>
+      <c r="B57" t="s">
+        <v>337</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="58" ht="79" customHeight="1" spans="1:6">
+      <c r="A58" t="s">
+        <v>342</v>
+      </c>
+      <c r="B58" t="s">
+        <v>343</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="59" ht="83" customHeight="1" spans="1:6">
+      <c r="A59" t="s">
+        <v>348</v>
+      </c>
+      <c r="B59" t="s">
+        <v>349</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="60" ht="79" customHeight="1" spans="1:6">
+      <c r="A60" t="s">
+        <v>354</v>
+      </c>
+      <c r="B60" t="s">
+        <v>355</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="61" ht="75" customHeight="1" spans="1:6">
+      <c r="A61" t="s">
+        <v>360</v>
+      </c>
+      <c r="B61" t="s">
+        <v>361</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="62" ht="80" customHeight="1" spans="1:6">
+      <c r="A62" t="s">
+        <v>366</v>
+      </c>
+      <c r="B62" t="s">
+        <v>367</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="63" ht="80" customHeight="1" spans="1:6">
+      <c r="A63" t="s">
+        <v>372</v>
+      </c>
+      <c r="B63" t="s">
+        <v>373</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="64" ht="85" customHeight="1" spans="1:6">
+      <c r="A64" t="s">
+        <v>378</v>
+      </c>
+      <c r="B64" t="s">
+        <v>379</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="65" ht="93" customHeight="1" spans="1:6">
+      <c r="A65" t="s">
+        <v>384</v>
+      </c>
+      <c r="B65" t="s">
+        <v>385</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="66" ht="78" customHeight="1" spans="1:6">
+      <c r="A66" t="s">
+        <v>390</v>
+      </c>
+      <c r="B66" t="s">
+        <v>391</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="67" ht="77" customHeight="1" spans="1:6">
+      <c r="A67" t="s">
+        <v>396</v>
+      </c>
+      <c r="B67" t="s">
+        <v>397</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="68" ht="79" customHeight="1" spans="1:6">
+      <c r="A68" t="s">
+        <v>402</v>
+      </c>
+      <c r="B68" t="s">
+        <v>403</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="69" ht="76" customHeight="1" spans="1:6">
+      <c r="A69" t="s">
+        <v>408</v>
+      </c>
+      <c r="B69" t="s">
+        <v>409</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="70" ht="87" customHeight="1" spans="1:6">
+      <c r="A70" t="s">
+        <v>414</v>
+      </c>
+      <c r="B70" t="s">
+        <v>415</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="71" ht="75" customHeight="1" spans="1:6">
+      <c r="A71" t="s">
+        <v>420</v>
+      </c>
+      <c r="B71" t="s">
+        <v>421</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="72" ht="81" customHeight="1" spans="1:6">
+      <c r="A72" t="s">
+        <v>426</v>
+      </c>
+      <c r="B72" t="s">
+        <v>427</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="73" ht="82" customHeight="1" spans="1:6">
+      <c r="A73" t="s">
+        <v>432</v>
+      </c>
+      <c r="B73" t="s">
+        <v>433</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="74" ht="77" customHeight="1" spans="1:6">
+      <c r="A74" t="s">
+        <v>438</v>
+      </c>
+      <c r="B74" t="s">
+        <v>439</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="75" ht="80" customHeight="1" spans="1:6">
+      <c r="A75" t="s">
+        <v>444</v>
+      </c>
+      <c r="B75" t="s">
+        <v>445</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="76" ht="77" customHeight="1" spans="1:6">
+      <c r="A76" t="s">
+        <v>450</v>
+      </c>
+      <c r="B76" t="s">
+        <v>451</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="F76" s="3" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="77" ht="77" customHeight="1" spans="1:6">
+      <c r="A77" t="s">
+        <v>456</v>
+      </c>
+      <c r="B77" t="s">
+        <v>457</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="F77" s="3" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="78" ht="82" customHeight="1" spans="1:6">
+      <c r="A78" t="s">
+        <v>462</v>
+      </c>
+      <c r="B78" t="s">
+        <v>463</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="F78" s="3" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="79" ht="84" customHeight="1" spans="1:6">
+      <c r="A79" t="s">
+        <v>468</v>
+      </c>
+      <c r="B79" t="s">
+        <v>469</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>471</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>472</v>
+      </c>
+      <c r="F79" s="3" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="80" ht="83" customHeight="1" spans="1:6">
+      <c r="A80" t="s">
+        <v>474</v>
+      </c>
+      <c r="B80" t="s">
+        <v>475</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="F80" s="3" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="81" ht="76" customHeight="1" spans="1:6">
+      <c r="A81" t="s">
+        <v>480</v>
+      </c>
+      <c r="B81" t="s">
+        <v>481</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>482</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>483</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="F81" s="3" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="82" ht="79" customHeight="1" spans="1:6">
+      <c r="A82" t="s">
+        <v>486</v>
+      </c>
+      <c r="B82" t="s">
+        <v>487</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="F82" s="3" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="83" ht="76" customHeight="1" spans="1:6">
+      <c r="A83" t="s">
+        <v>492</v>
+      </c>
+      <c r="B83" t="s">
+        <v>493</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>494</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>495</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="84" ht="78" customHeight="1" spans="1:6">
+      <c r="A84" t="s">
+        <v>498</v>
+      </c>
+      <c r="B84" t="s">
+        <v>499</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>500</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>501</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="F84" s="3" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="85" ht="79" customHeight="1" spans="1:6">
+      <c r="A85" t="s">
+        <v>504</v>
+      </c>
+      <c r="B85" t="s">
+        <v>505</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>506</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>507</v>
+      </c>
+      <c r="E85" s="3" t="s">
+        <v>508</v>
+      </c>
+      <c r="F85" s="3" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="86" ht="76" customHeight="1" spans="1:6">
+      <c r="A86" t="s">
+        <v>510</v>
+      </c>
+      <c r="B86" t="s">
+        <v>511</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>512</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>513</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="F86" s="3" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="87" ht="79" customHeight="1" spans="1:6">
+      <c r="A87" t="s">
+        <v>516</v>
+      </c>
+      <c r="B87" t="s">
+        <v>517</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>518</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>519</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="F87" s="3" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="88" ht="81" customHeight="1" spans="1:6">
+      <c r="A88" t="s">
+        <v>522</v>
+      </c>
+      <c r="B88" t="s">
+        <v>523</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>524</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="F88" s="3" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="89" ht="76" customHeight="1" spans="1:6">
+      <c r="A89" t="s">
+        <v>528</v>
+      </c>
+      <c r="B89" t="s">
+        <v>529</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>531</v>
+      </c>
+      <c r="E89" s="3" t="s">
+        <v>532</v>
+      </c>
+      <c r="F89" s="3" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="90" ht="76" customHeight="1" spans="1:6">
+      <c r="A90" t="s">
+        <v>534</v>
+      </c>
+      <c r="B90" t="s">
+        <v>535</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="F90" s="3" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="91" ht="83" customHeight="1" spans="1:6">
+      <c r="A91" t="s">
+        <v>540</v>
+      </c>
+      <c r="B91" t="s">
+        <v>541</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>542</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>543</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="F91" s="3" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="92" ht="75" customHeight="1" spans="1:6">
+      <c r="A92" t="s">
+        <v>546</v>
+      </c>
+      <c r="B92" t="s">
+        <v>547</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>549</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>550</v>
+      </c>
+      <c r="F92" s="3" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="93" ht="77" customHeight="1" spans="1:6">
+      <c r="A93" t="s">
+        <v>552</v>
+      </c>
+      <c r="B93" t="s">
+        <v>553</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>554</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>555</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="F93" s="3" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="94" ht="80" customHeight="1" spans="1:6">
+      <c r="A94" t="s">
+        <v>557</v>
+      </c>
+      <c r="B94" t="s">
+        <v>558</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>560</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="F94" s="3" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="95" ht="77" customHeight="1" spans="1:6">
+      <c r="A95" t="s">
+        <v>563</v>
+      </c>
+      <c r="B95" t="s">
+        <v>564</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>565</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="E95" s="3" t="s">
+        <v>567</v>
+      </c>
+      <c r="F95" s="3" t="s">
+        <v>568</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3586,27 +6678,27 @@
   <sheetData>
     <row r="1" customHeight="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>248</v>
+        <v>569</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
     <row r="2" customHeight="1" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>249</v>
+        <v>570</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
     <row r="3" customHeight="1" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>250</v>
+        <v>571</v>
       </c>
       <c r="B3" s="1"/>
     </row>
     <row r="4" customHeight="1" spans="1:1">
       <c r="A4" s="1" t="s">
-        <v>251</v>
+        <v>572</v>
       </c>
     </row>
   </sheetData>

</xml_diff>